<commit_message>
algorithm analysis update, new chunk sizes for makeMap
</commit_message>
<xml_diff>
--- a/Documents/MapAlgorithmAnalysis.xlsx
+++ b/Documents/MapAlgorithmAnalysis.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t># of subs</t>
   </si>
@@ -54,6 +54,21 @@
   </si>
   <si>
     <t>hours</t>
+  </si>
+  <si>
+    <t>Total distinct authors</t>
+  </si>
+  <si>
+    <t>Sum</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Running Total</t>
+  </si>
+  <si>
+    <t>Count</t>
   </si>
 </sst>
 </file>
@@ -112,694 +127,6 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Number</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> of Nodes vs Memory Usage</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.18111111111111111"/>
-          <c:y val="3.2407407407407406E-2"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$A$9:$A$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>2000</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8000</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$B$9:$B$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>65.242199999999997</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>65.918000000000006</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>66.234399999999994</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>66.519499999999994</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-5D23-4122-8358-9F83E8DE4D3E}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$A$9:$A$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>2000</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8000</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$C$9:$C$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>65.570300000000003</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>66.339799999999997</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>66.956999999999994</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>67</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-5D23-4122-8358-9F83E8DE4D3E}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="0.16133355205599301"/>
-                  <c:y val="-0.15319444444444444"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$A$9:$A$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>2000</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8000</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$D$9:$D$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>67.734399999999994</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>69.816400000000002</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>72.078100000000006</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>72.581999999999994</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-5D23-4122-8358-9F83E8DE4D3E}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="430594032"/>
-        <c:axId val="430594688"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="430594032"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Nodes</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US" baseline="0"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="430594688"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="430594688"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Memory Used (MiB)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="430594032"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1301,6 +628,360 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v># of subs</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0F74-4E07-834D-868DB3119E95}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="493921000"/>
+        <c:axId val="493920672"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="493921000"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="493920672"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="493920672"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="493921000"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2417,23 +2098,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>76199</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>241300</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>66674</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
+        <xdr:cNvPr id="8" name="Chart 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ABC0EF02-F3FE-491E-99AB-20D88E1C6326}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C86AEE94-2BE4-4418-A6F3-ADB5E0342E28}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2453,23 +2134,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>76199</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>66674</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>241300</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="8" name="Chart 7">
+        <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C86AEE94-2BE4-4418-A6F3-ADB5E0342E28}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00B837AC-350F-48C8-B6DA-5507CE7B544D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2787,10 +2468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2827,16 +2508,19 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="B2">
-        <v>65.293000000000006</v>
+        <v>0.1</v>
       </c>
       <c r="C2">
-        <v>65.293000000000006</v>
+        <v>29.6</v>
       </c>
       <c r="D2">
-        <v>65.293000000000006</v>
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
       </c>
       <c r="J2">
         <v>10</v>
@@ -2847,16 +2531,19 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>400</v>
+        <v>1000</v>
       </c>
       <c r="B3">
-        <v>65.800799999999995</v>
+        <v>0.1</v>
       </c>
       <c r="C3">
-        <v>65.800799999999995</v>
+        <v>29.9</v>
       </c>
       <c r="D3">
-        <v>65.949200000000005</v>
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>5703419</v>
       </c>
       <c r="J3">
         <v>100</v>
@@ -2867,16 +2554,16 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4">
-        <v>600</v>
+        <v>10000</v>
       </c>
       <c r="B4">
-        <v>65.011700000000005</v>
+        <v>1.2</v>
       </c>
       <c r="C4">
-        <v>65.011700000000005</v>
+        <v>37</v>
       </c>
       <c r="D4">
-        <v>65.8125</v>
+        <v>1</v>
       </c>
       <c r="J4">
         <v>1000</v>
@@ -2886,18 +2573,6 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A5">
-        <v>800</v>
-      </c>
-      <c r="B5">
-        <v>65.386700000000005</v>
-      </c>
-      <c r="C5">
-        <v>65.390600000000006</v>
-      </c>
-      <c r="D5">
-        <v>66.402299999999997</v>
-      </c>
       <c r="F5" t="s">
         <v>5</v>
       </c>
@@ -2909,18 +2584,6 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <v>1000</v>
-      </c>
-      <c r="B6">
-        <v>65.277299999999997</v>
-      </c>
-      <c r="C6">
-        <v>65.277299999999997</v>
-      </c>
-      <c r="D6">
-        <v>66.679699999999997</v>
-      </c>
       <c r="F6" s="1">
         <f>(0.0117*5703419 + 0.5)/(60^2)</f>
         <v>18.536250638888891</v>
@@ -2929,98 +2592,27 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D8" t="s">
-        <v>1</v>
-      </c>
-    </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A9">
-        <v>2000</v>
-      </c>
-      <c r="B9">
-        <v>65.242199999999997</v>
-      </c>
-      <c r="C9">
-        <v>65.570300000000003</v>
-      </c>
-      <c r="D9">
-        <v>67.734399999999994</v>
-      </c>
       <c r="F9" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A10">
-        <v>4000</v>
-      </c>
-      <c r="B10">
-        <v>65.918000000000006</v>
-      </c>
-      <c r="C10">
-        <v>66.339799999999997</v>
-      </c>
-      <c r="D10">
-        <v>69.816400000000002</v>
-      </c>
       <c r="F10">
-        <f>0.0008*(5703419) + 66.352</f>
-        <v>4629.0871999999999</v>
+        <f>(1*10^-8)*(F3/8)^2 - (1*10^-5)*F3/8 + 0.0011</f>
+        <v>5075.5262464939069</v>
       </c>
       <c r="G10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A11">
-        <v>6000</v>
-      </c>
-      <c r="B11">
-        <v>66.234399999999994</v>
-      </c>
-      <c r="C11">
-        <v>66.956999999999994</v>
-      </c>
-      <c r="D11">
-        <v>72.078100000000006</v>
-      </c>
       <c r="F11">
-        <v>4.85394973983</v>
+        <f>0.00104858*F10</f>
+        <v>5.3220953115485807</v>
       </c>
       <c r="G11" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A12">
-        <v>8000</v>
-      </c>
-      <c r="B12">
-        <v>66.519499999999994</v>
-      </c>
-      <c r="C12">
-        <v>67</v>
-      </c>
-      <c r="D12">
-        <v>72.581999999999994</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A13">
-        <v>10000</v>
-      </c>
-      <c r="B13">
-        <v>68.179699999999997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
switched to pandas, updated algorithm analysis
Using pandas to reduce memory usage substantially. Will need to adjust
for Unipartite casting now.
</commit_message>
<xml_diff>
--- a/Documents/MapAlgorithmAnalysis.xlsx
+++ b/Documents/MapAlgorithmAnalysis.xlsx
@@ -24,18 +24,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t># of subs</t>
-  </si>
-  <si>
-    <t>edge mem (MiB)</t>
-  </si>
-  <si>
-    <t>node mem (MiB)</t>
-  </si>
-  <si>
-    <t>query mem (MiB)</t>
   </si>
   <si>
     <t>Time(s)</t>
@@ -59,16 +50,7 @@
     <t>Total distinct authors</t>
   </si>
   <si>
-    <t>Sum</t>
-  </si>
-  <si>
-    <t>Average</t>
-  </si>
-  <si>
-    <t>Running Total</t>
-  </si>
-  <si>
-    <t>Count</t>
+    <t>Total Memory (MiB)</t>
   </si>
 </sst>
 </file>
@@ -291,20 +273,26 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$J$2:$J$5</c:f>
+              <c:f>Sheet1!$J$2:$J$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1000</c:v>
+                  <c:v>2000</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>10000</c:v>
                 </c:pt>
               </c:numCache>
@@ -312,21 +300,27 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$K$2:$K$5</c:f>
+              <c:f>Sheet1!$K$2:$K$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.79500000000000004</c:v>
+                  <c:v>2.7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.7949999999999999</c:v>
+                  <c:v>19.899999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11.8948914303073</c:v>
+                  <c:v>38.247</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>117.32</c:v>
+                  <c:v>99.1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>155.86000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>203.98</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -683,18 +677,20 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$1</c:f>
+              <c:f>Sheet1!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v># of subs</c:v>
+                  <c:v>Total Memory (MiB)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -724,11 +720,16 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="poly"/>
-            <c:order val="2"/>
+            <c:trendlineType val="linear"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.14096806649168853"/>
+                  <c:y val="-0.14856481481481482"/>
+                </c:manualLayout>
+              </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -761,10 +762,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$4</c:f>
+              <c:f>Sheet1!$A$2:$A$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>100</c:v>
                 </c:pt>
@@ -772,6 +773,15 @@
                   <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>10000</c:v>
                 </c:pt>
               </c:numCache>
@@ -779,18 +789,27 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$4</c:f>
+              <c:f>Sheet1!$B$2:$B$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>77</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>77.900000000000006</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>78.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>81.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>82.9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>83.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -798,7 +817,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-0F74-4E07-834D-868DB3119E95}"/>
+              <c16:uniqueId val="{00000000-0547-40B4-8808-9B79FCE63B12}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -810,11 +829,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="493921000"/>
-        <c:axId val="493920672"/>
+        <c:axId val="294203728"/>
+        <c:axId val="294206024"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="493921000"/>
+        <c:axId val="294203728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -871,12 +890,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="493920672"/>
+        <c:crossAx val="294206024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="493920672"/>
+        <c:axId val="294206024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -933,7 +952,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="493921000"/>
+        <c:crossAx val="294203728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2135,22 +2154,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>53975</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>31750</xdr:rowOff>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>241300</xdr:colOff>
+      <xdr:colOff>136525</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00B837AC-350F-48C8-B6DA-5507CE7B544D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A56A3806-D00E-4B05-8CE5-803F00D570B1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2471,13 +2490,13 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7265625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.90625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.6328125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="26.453125" bestFit="1" customWidth="1"/>
@@ -2491,19 +2510,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="J1" t="s">
         <v>0</v>
       </c>
       <c r="K1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
@@ -2511,22 +2524,16 @@
         <v>100</v>
       </c>
       <c r="B2">
-        <v>0.1</v>
-      </c>
-      <c r="C2">
-        <v>29.6</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
+        <v>77</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="J2">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="K2">
-        <v>0.79500000000000004</v>
+        <v>2.7</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
@@ -2534,85 +2541,105 @@
         <v>1000</v>
       </c>
       <c r="B3">
-        <v>0.1</v>
-      </c>
-      <c r="C3">
-        <v>29.9</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
+        <v>77.900000000000006</v>
       </c>
       <c r="F3">
         <v>5703419</v>
       </c>
       <c r="J3">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="K3">
-        <v>1.7949999999999999</v>
+        <v>19.899999999999999</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4">
-        <v>10000</v>
+        <v>2000</v>
       </c>
       <c r="B4">
-        <v>1.2</v>
-      </c>
-      <c r="C4">
-        <v>37</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
+        <v>78.3</v>
       </c>
       <c r="J4">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="K4">
-        <v>11.8948914303073</v>
+        <v>38.247</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>5000</v>
+      </c>
+      <c r="B5">
+        <v>81.3</v>
+      </c>
       <c r="F5" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="J5">
-        <v>10000</v>
+        <v>5000</v>
       </c>
       <c r="K5">
-        <v>117.32</v>
+        <v>99.1</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>8000</v>
+      </c>
+      <c r="B6">
+        <v>82.9</v>
+      </c>
       <c r="F6" s="1">
-        <f>(0.0117*5703419 + 0.5)/(60^2)</f>
-        <v>18.536250638888891</v>
+        <f>(0.0201*5703419-0.8159)/(60^2)</f>
+        <v>31.84386277777778</v>
       </c>
       <c r="G6" t="s">
-        <v>9</v>
+        <v>6</v>
+      </c>
+      <c r="J6">
+        <v>8000</v>
+      </c>
+      <c r="K6">
+        <v>155.86000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>10000</v>
+      </c>
+      <c r="B7">
+        <v>83.1</v>
+      </c>
+      <c r="J7">
+        <v>10000</v>
+      </c>
+      <c r="K7">
+        <v>203.98</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="F9" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="F10">
-        <f>(1*10^-8)*(F3/8)^2 - (1*10^-5)*F3/8 + 0.0011</f>
-        <v>5075.5262464939069</v>
+        <f>0.0007*F3 + 77.233</f>
+        <v>4069.6263000000004</v>
       </c>
       <c r="G10" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="F11">
         <f>0.00104858*F10</f>
-        <v>5.3220953115485807</v>
+        <v>4.2673287456539999</v>
       </c>
       <c r="G11" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>